<commit_message>
Sprint backlog updated (acceptance criteria, descriptions, ordering)
</commit_message>
<xml_diff>
--- a/doc/_scrum/scrum_team_yellow.xlsx
+++ b/doc/_scrum/scrum_team_yellow.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26915"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevin/Dropbox/Lerngruppe_Share/Software_Engineering_and_Design/gruppenarbeit/Implementation/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14600" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="14595" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectTeam" sheetId="3" r:id="rId1"/>
@@ -21,11 +16,8 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Product Backlog'!$A$1:$H$16</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Sprint Backlog'!$A$1:$M$1</definedName>
   </definedNames>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -34,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="121">
   <si>
     <t>ID</t>
   </si>
@@ -220,9 +212,6 @@
   </si>
   <si>
     <t>Navigation between views, base layout</t>
-  </si>
-  <si>
-    <t>Create patient view</t>
   </si>
   <si>
     <t>UI</t>
@@ -302,9 +291,6 @@
     <t>michel, kevin</t>
   </si>
   <si>
-    <t>assigned</t>
-  </si>
-  <si>
     <t>layout lead</t>
   </si>
   <si>
@@ -381,9 +367,6 @@
     <t>all</t>
   </si>
   <si>
-    <t>done</t>
-  </si>
-  <si>
     <t>Comment</t>
   </si>
   <si>
@@ -393,13 +376,25 @@
     <t>Create prescription</t>
   </si>
   <si>
-    <t>Create medicaments tile</t>
-  </si>
-  <si>
     <t>michel</t>
   </si>
   <si>
-    <t>Create medicaments model &amp; DTO</t>
+    <t>* ability to navigate between pages via menu</t>
+  </si>
+  <si>
+    <t>* ability to prescribe a new medicament for a patient</t>
+  </si>
+  <si>
+    <t>Create search bar and menu</t>
+  </si>
+  <si>
+    <t>Create prescriptions tile</t>
+  </si>
+  <si>
+    <t>Create prescriptions model</t>
+  </si>
+  <si>
+    <t>Create prescriptions presenter</t>
   </si>
 </sst>
 </file>
@@ -498,11 +493,11 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Stand." xfId="0" builtinId="0"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yy"/>
+      <numFmt numFmtId="164" formatCode="dd/mm/yy"/>
     </dxf>
     <dxf>
       <font>
@@ -542,10 +537,10 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A1:M14" totalsRowCount="1" headerRowDxfId="1">
-  <autoFilter ref="A1:M13"/>
-  <sortState ref="A2:M13">
-    <sortCondition ref="L1:L13"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A1:M15" totalsRowCount="1" headerRowDxfId="1">
+  <autoFilter ref="A1:M14"/>
+  <sortState ref="A2:M14">
+    <sortCondition ref="H1:H14"/>
   </sortState>
   <tableColumns count="13">
     <tableColumn id="1" name="User Story ID" totalsRowLabel="Total"/>
@@ -859,14 +854,14 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="64.5" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="75" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="3" customFormat="1" ht="19.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" s="3" customFormat="1" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -874,7 +869,7 @@
         <v>12</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -885,7 +880,7 @@
         <v>28</v>
       </c>
       <c r="C2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -896,7 +891,7 @@
         <v>26</v>
       </c>
       <c r="C3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -907,7 +902,7 @@
         <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -918,7 +913,7 @@
         <v>27</v>
       </c>
       <c r="C5" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -929,7 +924,7 @@
         <v>24</v>
       </c>
       <c r="C6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -940,55 +935,55 @@
         <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B9" s="7" t="s">
         <v>81</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B13" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
   </sheetData>
@@ -1000,21 +995,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView zoomScale="152" zoomScaleNormal="152" zoomScalePageLayoutView="152" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+    <sheetView tabSelected="1" zoomScale="152" zoomScaleNormal="152" zoomScalePageLayoutView="152" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.6640625" customWidth="1"/>
-    <col min="2" max="2" width="31.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="41.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="17.33203125" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" customWidth="1"/>
-    <col min="6" max="6" width="13.1640625" customWidth="1"/>
-    <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.5" customWidth="1"/>
-    <col min="9" max="9" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.7109375" customWidth="1"/>
+    <col min="2" max="2" width="37.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.5703125" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.42578125" customWidth="1"/>
+    <col min="9" max="9" width="48.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.2">
@@ -1028,13 +1023,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>10</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>8</v>
@@ -1043,10 +1038,10 @@
         <v>4</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1057,7 +1052,7 @@
         <v>29</v>
       </c>
       <c r="D2" s="1">
-        <v>10</v>
+        <v>999</v>
       </c>
       <c r="E2" s="1">
         <v>16</v>
@@ -1069,13 +1064,13 @@
         <v>0</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>55</v>
+        <v>108</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>4</v>
       </c>
@@ -1083,10 +1078,10 @@
         <v>52</v>
       </c>
       <c r="C3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D3" s="1">
-        <v>8</v>
+        <v>998</v>
       </c>
       <c r="E3">
         <v>16</v>
@@ -1098,24 +1093,24 @@
         <v>0</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>55</v>
+        <v>108</v>
       </c>
       <c r="I3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C4" t="s">
         <v>61</v>
       </c>
       <c r="D4" s="1">
-        <v>7</v>
+        <v>997</v>
       </c>
       <c r="E4">
         <v>16</v>
@@ -1127,21 +1122,24 @@
         <v>0</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+        <v>108</v>
+      </c>
+      <c r="I4" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>113</v>
       </c>
       <c r="C5" t="s">
-        <v>62</v>
+        <v>44</v>
       </c>
       <c r="D5" s="1">
-        <v>6</v>
+        <v>996</v>
       </c>
       <c r="E5">
         <v>4</v>
@@ -1153,18 +1151,21 @@
         <v>0</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="1">
-        <v>3</v>
+        <v>108</v>
+      </c>
+      <c r="I5" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C6" t="s">
-        <v>33</v>
+        <v>117</v>
       </c>
       <c r="D6" s="1">
         <v>1</v>
@@ -1182,15 +1183,15 @@
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C7" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="D7" s="1">
         <v>1</v>
@@ -1208,15 +1209,15 @@
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>6</v>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D8" s="1">
         <v>1</v>
@@ -1234,15 +1235,15 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="1">
-        <v>7</v>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>115</v>
+        <v>38</v>
       </c>
       <c r="C9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D9" s="1">
         <v>1</v>
@@ -1260,15 +1261,15 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>8</v>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D10" s="1">
         <v>1</v>
@@ -1286,7 +1287,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1312,7 +1313,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1338,7 +1339,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1364,7 +1365,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1390,7 +1391,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1416,7 +1417,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1461,32 +1462,32 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M14"/>
+  <dimension ref="A1:M15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="146" zoomScaleNormal="146" zoomScalePageLayoutView="146" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView zoomScale="146" zoomScaleNormal="146" zoomScalePageLayoutView="146" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.1640625" customWidth="1"/>
-    <col min="3" max="3" width="27" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.5" customWidth="1"/>
-    <col min="5" max="5" width="13.6640625" customWidth="1"/>
-    <col min="6" max="6" width="12.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.6640625" customWidth="1"/>
-    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.6640625" customWidth="1"/>
-    <col min="10" max="10" width="17.6640625" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="39.1640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.140625" customWidth="1"/>
+    <col min="3" max="3" width="32.140625" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.7109375" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.7109375" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.7109375" customWidth="1"/>
+    <col min="10" max="10" width="17.7109375" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="43.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="4" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>6</v>
@@ -1495,13 +1496,13 @@
         <v>1</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>7</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>11</v>
@@ -1510,349 +1511,349 @@
         <v>3</v>
       </c>
       <c r="I1" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="K1" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="J1" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>107</v>
-      </c>
       <c r="L1" s="9" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="M1" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>11</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F2" t="s">
+        <v>86</v>
+      </c>
+      <c r="G2" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="H2" t="s">
+        <v>71</v>
+      </c>
+      <c r="I2">
+        <v>8</v>
+      </c>
+      <c r="L2" t="s">
+        <v>108</v>
+      </c>
+      <c r="M2" s="6">
+        <v>42504</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>11</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E3" t="s">
+        <v>62</v>
+      </c>
+      <c r="F3" t="s">
+        <v>75</v>
+      </c>
+      <c r="G3" t="s">
+        <v>110</v>
+      </c>
+      <c r="H3" t="s">
+        <v>71</v>
+      </c>
+      <c r="I3">
+        <v>8</v>
+      </c>
+      <c r="L3" t="s">
+        <v>108</v>
+      </c>
+      <c r="M3" s="6">
+        <v>42504</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
         <v>54</v>
       </c>
-      <c r="E2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F2" t="s">
-        <v>111</v>
-      </c>
-      <c r="G2" t="s">
-        <v>76</v>
-      </c>
-      <c r="H2" t="s">
-        <v>73</v>
-      </c>
-      <c r="I2">
-        <v>6</v>
-      </c>
-      <c r="L2" t="s">
-        <v>88</v>
-      </c>
-      <c r="M2" s="6">
-        <v>42505</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>53</v>
-      </c>
-      <c r="D3" s="2"/>
-      <c r="E3" t="s">
-        <v>9</v>
-      </c>
-      <c r="F3" t="s">
-        <v>111</v>
-      </c>
-      <c r="G3" t="s">
-        <v>97</v>
-      </c>
-      <c r="H3" t="s">
-        <v>73</v>
-      </c>
-      <c r="I3">
-        <v>2</v>
-      </c>
-      <c r="L3" t="s">
-        <v>88</v>
-      </c>
-      <c r="M3" s="6">
-        <v>42512</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>1</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
-      </c>
-      <c r="C4" t="s">
-        <v>56</v>
-      </c>
       <c r="E4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F4" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="G4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I4">
         <v>6</v>
       </c>
       <c r="L4" t="s">
-        <v>88</v>
+        <v>108</v>
       </c>
       <c r="M4" s="6">
-        <v>42512</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+        <v>42505</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>117</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="D5" s="2"/>
       <c r="E5" t="s">
-        <v>63</v>
+        <v>9</v>
       </c>
       <c r="F5" t="s">
-        <v>97</v>
+        <v>109</v>
       </c>
       <c r="G5" t="s">
-        <v>118</v>
+        <v>95</v>
       </c>
       <c r="H5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I5">
         <v>2</v>
       </c>
       <c r="L5" t="s">
-        <v>88</v>
+        <v>108</v>
       </c>
       <c r="M5" s="6">
         <v>42512</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="B6">
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>119</v>
+        <v>56</v>
       </c>
       <c r="E6" t="s">
-        <v>9</v>
+        <v>63</v>
       </c>
       <c r="F6" t="s">
-        <v>97</v>
+        <v>109</v>
       </c>
       <c r="G6" t="s">
-        <v>118</v>
+        <v>75</v>
       </c>
       <c r="H6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I6">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="L6" t="s">
-        <v>88</v>
+        <v>108</v>
       </c>
       <c r="M6" s="6">
         <v>42512</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B7">
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>93</v>
-      </c>
-      <c r="D7" t="s">
-        <v>68</v>
+        <v>118</v>
       </c>
       <c r="E7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F7" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="G7" t="s">
-        <v>76</v>
+        <v>114</v>
       </c>
       <c r="H7" t="s">
         <v>72</v>
       </c>
       <c r="I7">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="L7" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="M7" s="6">
-        <v>42504</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+        <v>42512</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>1</v>
+        <v>14</v>
       </c>
       <c r="B8">
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>98</v>
+        <v>119</v>
       </c>
       <c r="E8" t="s">
         <v>9</v>
       </c>
       <c r="F8" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="G8" t="s">
-        <v>109</v>
+        <v>114</v>
       </c>
       <c r="H8" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L8" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="M8" s="6">
         <v>42512</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="B9">
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>60</v>
-      </c>
-      <c r="D9" t="s">
-        <v>68</v>
+        <v>120</v>
       </c>
       <c r="E9" t="s">
         <v>63</v>
       </c>
       <c r="F9" t="s">
-        <v>76</v>
+        <v>95</v>
       </c>
       <c r="G9" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="H9" t="s">
         <v>72</v>
       </c>
       <c r="I9">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="L9" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="M9" s="6">
-        <v>42504</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+        <v>42512</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="B10">
         <v>1</v>
       </c>
       <c r="C10" t="s">
+        <v>96</v>
+      </c>
+      <c r="E10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F10" t="s">
         <v>95</v>
       </c>
-      <c r="E10" t="s">
-        <v>96</v>
-      </c>
-      <c r="F10" t="s">
-        <v>97</v>
-      </c>
       <c r="G10" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="H10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I10">
         <v>2</v>
       </c>
       <c r="L10" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="M10" s="6">
-        <v>42505</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+        <v>42512</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B11">
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>59</v>
+        <v>93</v>
       </c>
       <c r="E11" t="s">
-        <v>63</v>
+        <v>94</v>
       </c>
       <c r="F11" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="G11" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="H11" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I11">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="L11" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="M11" s="6">
         <v>42505</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>4</v>
       </c>
@@ -1860,31 +1861,31 @@
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="E12" t="s">
-        <v>9</v>
+        <v>62</v>
       </c>
       <c r="F12" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="G12" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="H12" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I12">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="L12" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="M12" s="6">
-        <v>42512</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+        <v>42505</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>4</v>
       </c>
@@ -1892,35 +1893,67 @@
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="E13" t="s">
-        <v>64</v>
+        <v>9</v>
       </c>
       <c r="F13" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="G13" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="H13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="I13">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="L13" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="M13" s="6">
         <v>42512</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>100</v>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>4</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>58</v>
+      </c>
+      <c r="E14" t="s">
+        <v>63</v>
+      </c>
+      <c r="F14" t="s">
+        <v>97</v>
+      </c>
+      <c r="G14" t="s">
+        <v>107</v>
+      </c>
+      <c r="H14" t="s">
+        <v>72</v>
       </c>
       <c r="I14">
+        <v>6</v>
+      </c>
+      <c r="L14" t="s">
+        <v>108</v>
+      </c>
+      <c r="M14" s="6">
+        <v>42512</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>98</v>
+      </c>
+      <c r="I15">
         <f>SUBTOTAL(109,Tabelle1[Planned effort])</f>
         <v>52</v>
       </c>
@@ -1941,14 +1974,14 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" customWidth="1"/>
-    <col min="4" max="4" width="14.33203125" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="5" customFormat="1" ht="26.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" s="5" customFormat="1" ht="26.85" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>13</v>
       </c>

</xml_diff>

<commit_message>
product/sprint backlog updated, presentation review meeting 1
</commit_message>
<xml_diff>
--- a/doc/_scrum/scrum_team_yellow.xlsx
+++ b/doc/_scrum/scrum_team_yellow.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="26915"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevin/Dropbox/Lerngruppe_Share/Software_Engineering_and_Design/gruppenarbeit/Implementation/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="25605" windowHeight="14595" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14580" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectTeam" sheetId="3" r:id="rId1"/>
@@ -16,8 +21,11 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Product Backlog'!$A$1:$H$16</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Sprint Backlog'!$A$1:$M$1</definedName>
   </definedNames>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -26,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="144">
   <si>
     <t>ID</t>
   </si>
@@ -121,15 +129,9 @@
     <t>Patient search</t>
   </si>
   <si>
-    <t>Patient history</t>
-  </si>
-  <si>
     <t>Escalation</t>
   </si>
   <si>
-    <t>Show illness history of patient</t>
-  </si>
-  <si>
     <t>Edit patient base data</t>
   </si>
   <si>
@@ -148,9 +150,6 @@
     <t>Connect external systems</t>
   </si>
   <si>
-    <t>Responsive Design</t>
-  </si>
-  <si>
     <t>Create a new wiki article</t>
   </si>
   <si>
@@ -176,9 +175,6 @@
   </si>
   <si>
     <t>Connect medication DB and illness DB</t>
-  </si>
-  <si>
-    <t>Enable support for mobile clients</t>
   </si>
   <si>
     <t>Patient overview - base data</t>
@@ -385,9 +381,6 @@
     <t>* ability to prescribe a new medicament for a patient</t>
   </si>
   <si>
-    <t>Create search bar and menu</t>
-  </si>
-  <si>
     <t>Create prescriptions tile</t>
   </si>
   <si>
@@ -395,13 +388,97 @@
   </si>
   <si>
     <t>Create prescriptions presenter</t>
+  </si>
+  <si>
+    <t>done</t>
+  </si>
+  <si>
+    <t>Make Prescriptions persistable</t>
+  </si>
+  <si>
+    <t>Person search view</t>
+  </si>
+  <si>
+    <t>Person search controller</t>
+  </si>
+  <si>
+    <t>Person search model</t>
+  </si>
+  <si>
+    <t>Show meeting history in patient overview</t>
+  </si>
+  <si>
+    <t>Improve look &amp; feel of application</t>
+  </si>
+  <si>
+    <t>* ability to search for name and/or birthdate</t>
+  </si>
+  <si>
+    <t>Adapt UML diagram</t>
+  </si>
+  <si>
+    <t>Only model layer</t>
+  </si>
+  <si>
+    <t>Show meeting history of patient</t>
+  </si>
+  <si>
+    <t>Meeting patient history</t>
+  </si>
+  <si>
+    <t>Improve look &amp; feel of UI (customer feedback)</t>
+  </si>
+  <si>
+    <t>Task 12</t>
+  </si>
+  <si>
+    <t>Adapt UML diagram according to code</t>
+  </si>
+  <si>
+    <t>Task 13</t>
+  </si>
+  <si>
+    <t>Introduce state pattern</t>
+  </si>
+  <si>
+    <t>Remove person inheritance</t>
+  </si>
+  <si>
+    <t>Connect with meeting view</t>
+  </si>
+  <si>
+    <t>Allow meeting to have different states</t>
+  </si>
+  <si>
+    <t>Model &amp; Controller</t>
+  </si>
+  <si>
+    <t>Indicate meeting states in GUI</t>
+  </si>
+  <si>
+    <t>alex, simon</t>
+  </si>
+  <si>
+    <t>Improve usability &amp; menu</t>
+  </si>
+  <si>
+    <t>assigned</t>
+  </si>
+  <si>
+    <t>Allow to search for patients</t>
+  </si>
+  <si>
+    <t>Connect with patient overview</t>
+  </si>
+  <si>
+    <t>Read real patient data from database</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -429,6 +506,22 @@
       <b/>
       <sz val="10"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -463,8 +556,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -492,12 +589,16 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+  <cellStyles count="5">
+    <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Stand." xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
-      <numFmt numFmtId="164" formatCode="dd/mm/yy"/>
+      <numFmt numFmtId="19" formatCode="dd/mm/yy"/>
     </dxf>
     <dxf>
       <font>
@@ -537,8 +638,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A1:M15" totalsRowCount="1" headerRowDxfId="1">
-  <autoFilter ref="A1:M14"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A1:M25" totalsRowCount="1" headerRowDxfId="1">
+  <autoFilter ref="A1:M24">
+    <filterColumn colId="1">
+      <filters>
+        <filter val="2"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <sortState ref="A2:M14">
     <sortCondition ref="H1:H14"/>
   </sortState>
@@ -850,18 +957,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView zoomScale="148" zoomScaleNormal="148" zoomScalePageLayoutView="148" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScale="148" zoomScaleNormal="148" zoomScalePageLayoutView="148" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="75" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="17.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="3" customFormat="1" ht="19.350000000000001" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" s="3" customFormat="1" ht="19.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
@@ -869,7 +976,7 @@
         <v>12</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -880,7 +987,7 @@
         <v>28</v>
       </c>
       <c r="C2" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -891,7 +998,7 @@
         <v>26</v>
       </c>
       <c r="C3" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -902,7 +1009,7 @@
         <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -913,7 +1020,7 @@
         <v>27</v>
       </c>
       <c r="C5" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -924,7 +1031,7 @@
         <v>24</v>
       </c>
       <c r="C6" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -935,55 +1042,55 @@
         <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="B10" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B13" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -995,21 +1102,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="152" zoomScaleNormal="152" zoomScalePageLayoutView="152" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView zoomScale="142" zoomScaleNormal="142" zoomScalePageLayoutView="142" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" customWidth="1"/>
-    <col min="2" max="2" width="37.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42.5703125" customWidth="1"/>
-    <col min="4" max="4" width="18.85546875" customWidth="1"/>
-    <col min="5" max="5" width="11.7109375" customWidth="1"/>
-    <col min="6" max="6" width="13.140625" customWidth="1"/>
-    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.42578125" customWidth="1"/>
-    <col min="9" max="9" width="48.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.6640625" customWidth="1"/>
+    <col min="2" max="2" width="37.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.5" customWidth="1"/>
+    <col min="4" max="4" width="18.83203125" customWidth="1"/>
+    <col min="5" max="5" width="11.6640625" customWidth="1"/>
+    <col min="6" max="6" width="13.1640625" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.5" customWidth="1"/>
+    <col min="9" max="9" width="48.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.2">
@@ -1023,13 +1130,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>10</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>8</v>
@@ -1038,15 +1145,15 @@
         <v>4</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>29</v>
@@ -1061,24 +1168,24 @@
         <v>0</v>
       </c>
       <c r="G2" s="1">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="C3" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D3" s="1">
         <v>998</v>
@@ -1090,24 +1197,24 @@
         <v>0</v>
       </c>
       <c r="G3" s="1">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="I3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C4" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D4" s="1">
         <v>997</v>
@@ -1119,24 +1226,24 @@
         <v>0</v>
       </c>
       <c r="G4" s="1">
-        <v>0</v>
+        <v>16</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="I4" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D5" s="1">
         <v>996</v>
@@ -1151,308 +1258,357 @@
         <v>0</v>
       </c>
       <c r="H5" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="I5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>16</v>
+      </c>
+      <c r="B6" t="s">
+        <v>129</v>
+      </c>
+      <c r="C6" t="s">
+        <v>130</v>
+      </c>
+      <c r="D6" s="1">
+        <v>995</v>
+      </c>
+      <c r="E6">
+        <v>4</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0</v>
+      </c>
+      <c r="G6" s="1">
+        <v>0</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="I6" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>17</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="D7" s="1">
+        <v>994</v>
+      </c>
+      <c r="E7">
+        <v>20</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>2</v>
+      </c>
+      <c r="B8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C8" t="s">
+        <v>141</v>
+      </c>
+      <c r="D8" s="1">
+        <v>993</v>
+      </c>
+      <c r="E8">
+        <v>12</v>
+      </c>
+      <c r="F8" s="1">
+        <v>0</v>
+      </c>
+      <c r="G8" s="1">
+        <v>0</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>3</v>
+      </c>
+      <c r="B9" t="s">
+        <v>127</v>
+      </c>
+      <c r="C9" t="s">
+        <v>126</v>
+      </c>
+      <c r="D9" s="1">
+        <v>992</v>
+      </c>
+      <c r="E9">
+        <v>20</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>15</v>
+      </c>
+      <c r="B10" t="s">
+        <v>128</v>
+      </c>
+      <c r="C10" t="s">
+        <v>139</v>
+      </c>
+      <c r="D10" s="1">
+        <v>991</v>
+      </c>
+      <c r="E10">
+        <v>6</v>
+      </c>
+      <c r="F10" s="1">
+        <v>0</v>
+      </c>
+      <c r="G10" s="1">
+        <v>0</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>5</v>
+      </c>
+      <c r="B11" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" s="1">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11" s="1">
+        <v>0</v>
+      </c>
+      <c r="G11" s="1">
+        <v>0</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>6</v>
+      </c>
+      <c r="B12" t="s">
+        <v>36</v>
+      </c>
+      <c r="C12" t="s">
+        <v>39</v>
+      </c>
+      <c r="D12" s="1">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12" s="1">
+        <v>0</v>
+      </c>
+      <c r="G12" s="1">
+        <v>0</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>7</v>
+      </c>
+      <c r="B13" t="s">
         <v>108</v>
       </c>
-      <c r="I5" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>2</v>
-      </c>
-      <c r="B6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C6" t="s">
-        <v>117</v>
-      </c>
-      <c r="D6" s="1">
-        <v>1</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-      <c r="F6" s="1">
-        <v>0</v>
-      </c>
-      <c r="G6" s="1">
-        <v>0</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="1">
-        <v>3</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="C13" t="s">
+        <v>40</v>
+      </c>
+      <c r="D13" s="1">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13" s="1">
+        <v>0</v>
+      </c>
+      <c r="G13" s="1">
+        <v>0</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>9</v>
+      </c>
+      <c r="B14" t="s">
         <v>31</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C14" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="1">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14" s="1">
+        <v>0</v>
+      </c>
+      <c r="G14" s="1">
+        <v>0</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>10</v>
+      </c>
+      <c r="B15" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" s="1">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+      <c r="F15" s="1">
+        <v>0</v>
+      </c>
+      <c r="G15" s="1">
+        <v>0</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>12</v>
+      </c>
+      <c r="B16" t="s">
         <v>33</v>
       </c>
-      <c r="D7" s="1">
-        <v>1</v>
-      </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-      <c r="F7" s="1">
-        <v>0</v>
-      </c>
-      <c r="G7" s="1">
-        <v>0</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="1">
-        <v>5</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="C16" t="s">
+        <v>44</v>
+      </c>
+      <c r="D16" s="1">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+      <c r="F16" s="1">
+        <v>0</v>
+      </c>
+      <c r="G16" s="1">
+        <v>0</v>
+      </c>
+      <c r="H16" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <v>13</v>
+      </c>
+      <c r="B17" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" t="s">
+        <v>45</v>
+      </c>
+      <c r="D17" s="1">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17" s="1">
+        <v>0</v>
+      </c>
+      <c r="G17" s="1">
+        <v>0</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>14</v>
+      </c>
+      <c r="B18" t="s">
         <v>37</v>
       </c>
-      <c r="C8" t="s">
-        <v>41</v>
-      </c>
-      <c r="D8" s="1">
-        <v>1</v>
-      </c>
-      <c r="E8">
-        <v>0</v>
-      </c>
-      <c r="F8" s="1">
-        <v>0</v>
-      </c>
-      <c r="G8" s="1">
-        <v>0</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>6</v>
-      </c>
-      <c r="B9" t="s">
-        <v>38</v>
-      </c>
-      <c r="C9" t="s">
-        <v>42</v>
-      </c>
-      <c r="D9" s="1">
-        <v>1</v>
-      </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-      <c r="F9" s="1">
-        <v>0</v>
-      </c>
-      <c r="G9" s="1">
-        <v>0</v>
-      </c>
-      <c r="H9" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="1">
-        <v>7</v>
-      </c>
-      <c r="B10" t="s">
-        <v>112</v>
-      </c>
-      <c r="C10" t="s">
-        <v>43</v>
-      </c>
-      <c r="D10" s="1">
-        <v>1</v>
-      </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-      <c r="F10" s="1">
-        <v>0</v>
-      </c>
-      <c r="G10" s="1">
-        <v>0</v>
-      </c>
-      <c r="H10" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="1">
-        <v>9</v>
-      </c>
-      <c r="B11" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" t="s">
-        <v>45</v>
-      </c>
-      <c r="D11" s="1">
-        <v>1</v>
-      </c>
-      <c r="E11">
-        <v>0</v>
-      </c>
-      <c r="F11" s="1">
-        <v>0</v>
-      </c>
-      <c r="G11" s="1">
-        <v>0</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>10</v>
-      </c>
-      <c r="B12" t="s">
-        <v>34</v>
-      </c>
-      <c r="C12" t="s">
+      <c r="C18" t="s">
         <v>46</v>
       </c>
-      <c r="D12" s="1">
-        <v>1</v>
-      </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-      <c r="F12" s="1">
-        <v>0</v>
-      </c>
-      <c r="G12" s="1">
-        <v>0</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>35</v>
-      </c>
-      <c r="C13" t="s">
-        <v>47</v>
-      </c>
-      <c r="D13" s="1">
-        <v>1</v>
-      </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-      <c r="F13" s="1">
-        <v>0</v>
-      </c>
-      <c r="G13" s="1">
-        <v>0</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="1">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>36</v>
-      </c>
-      <c r="C14" t="s">
-        <v>48</v>
-      </c>
-      <c r="D14" s="1">
-        <v>1</v>
-      </c>
-      <c r="E14">
-        <v>0</v>
-      </c>
-      <c r="F14" s="1">
-        <v>0</v>
-      </c>
-      <c r="G14" s="1">
-        <v>0</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>39</v>
-      </c>
-      <c r="C15" t="s">
-        <v>49</v>
-      </c>
-      <c r="D15" s="1">
-        <v>1</v>
-      </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
-      <c r="F15" s="1">
-        <v>0</v>
-      </c>
-      <c r="G15" s="1">
-        <v>0</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="1">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>40</v>
-      </c>
-      <c r="C16" t="s">
-        <v>50</v>
-      </c>
-      <c r="D16" s="1">
-        <v>1</v>
-      </c>
-      <c r="E16">
-        <v>0</v>
-      </c>
-      <c r="F16" s="1">
-        <v>0</v>
-      </c>
-      <c r="G16" s="1">
-        <v>0</v>
-      </c>
-      <c r="H16" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="1"/>
+      <c r="D18" s="1">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18" s="1">
+        <v>0</v>
+      </c>
+      <c r="G18" s="1">
+        <v>0</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>51</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:H16">
-    <sortState ref="A2:H16">
-      <sortCondition descending="1" ref="D1:D16"/>
+    <sortState ref="A2:H18">
+      <sortCondition descending="1" ref="D1:D18"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1462,32 +1618,32 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M15"/>
+  <dimension ref="A1:M25"/>
   <sheetViews>
-    <sheetView zoomScale="146" zoomScaleNormal="146" zoomScalePageLayoutView="146" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView tabSelected="1" zoomScale="139" zoomScaleNormal="139" zoomScalePageLayoutView="139" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.140625" customWidth="1"/>
-    <col min="3" max="3" width="32.140625" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" customWidth="1"/>
-    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.7109375" customWidth="1"/>
-    <col min="8" max="8" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.7109375" customWidth="1"/>
-    <col min="10" max="10" width="17.7109375" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="43.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.1640625" customWidth="1"/>
+    <col min="3" max="3" width="32.1640625" customWidth="1"/>
+    <col min="4" max="4" width="24" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" customWidth="1"/>
+    <col min="8" max="8" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.6640625" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="39.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="4" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>6</v>
@@ -1496,13 +1652,13 @@
         <v>1</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>7</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>11</v>
@@ -1511,22 +1667,22 @@
         <v>3</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="L1" s="9" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>11</v>
       </c>
@@ -1534,34 +1690,34 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F2" t="s">
+        <v>82</v>
+      </c>
+      <c r="G2" t="s">
+        <v>71</v>
+      </c>
+      <c r="H2" t="s">
         <v>67</v>
-      </c>
-      <c r="E2" t="s">
-        <v>62</v>
-      </c>
-      <c r="F2" t="s">
-        <v>86</v>
-      </c>
-      <c r="G2" t="s">
-        <v>75</v>
-      </c>
-      <c r="H2" t="s">
-        <v>71</v>
       </c>
       <c r="I2">
         <v>8</v>
       </c>
       <c r="L2" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="M2" s="6">
         <v>42504</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>11</v>
       </c>
@@ -1569,34 +1725,37 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="D3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E3" t="s">
+        <v>58</v>
+      </c>
+      <c r="F3" t="s">
+        <v>71</v>
+      </c>
+      <c r="G3" t="s">
+        <v>106</v>
+      </c>
+      <c r="H3" t="s">
         <v>67</v>
-      </c>
-      <c r="E3" t="s">
-        <v>62</v>
-      </c>
-      <c r="F3" t="s">
-        <v>75</v>
-      </c>
-      <c r="G3" t="s">
-        <v>110</v>
-      </c>
-      <c r="H3" t="s">
-        <v>71</v>
       </c>
       <c r="I3">
         <v>8</v>
       </c>
+      <c r="K3">
+        <v>4</v>
+      </c>
       <c r="L3" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="M3" s="6">
         <v>42504</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1604,31 +1763,31 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="E4" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F4" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="G4" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="H4" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="I4">
         <v>6</v>
       </c>
       <c r="L4" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="M4" s="6">
         <v>42505</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1636,32 +1795,32 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" t="s">
         <v>9</v>
       </c>
       <c r="F5" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="G5" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="H5" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="I5">
         <v>2</v>
       </c>
       <c r="L5" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="M5" s="6">
         <v>42512</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -1669,31 +1828,31 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="E6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="F6" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="G6" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="H6" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="I6">
         <v>6</v>
       </c>
       <c r="L6" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="M6" s="6">
         <v>42512</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>14</v>
       </c>
@@ -1701,31 +1860,31 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="E7" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F7" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="G7" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="H7" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="I7">
         <v>2</v>
       </c>
       <c r="L7" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="M7" s="6">
         <v>42512</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>14</v>
       </c>
@@ -1733,31 +1892,31 @@
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="E8" t="s">
         <v>9</v>
       </c>
       <c r="F8" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="G8" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="H8" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="I8">
         <v>1</v>
       </c>
       <c r="L8" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="M8" s="6">
         <v>42512</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>14</v>
       </c>
@@ -1765,31 +1924,31 @@
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="E9" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="F9" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="G9" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="H9" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="I9">
         <v>1</v>
       </c>
       <c r="L9" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="M9" s="6">
         <v>42512</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1</v>
       </c>
@@ -1797,31 +1956,31 @@
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="E10" t="s">
         <v>9</v>
       </c>
       <c r="F10" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="G10" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="H10" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="I10">
         <v>2</v>
       </c>
       <c r="L10" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="M10" s="6">
         <v>42512</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>11</v>
       </c>
@@ -1829,31 +1988,31 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="E11" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="F11" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="G11" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="H11" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="I11">
         <v>2</v>
       </c>
       <c r="L11" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="M11" s="6">
         <v>42505</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>4</v>
       </c>
@@ -1861,31 +2020,34 @@
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="E12" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F12" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="G12" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="H12" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="I12">
         <v>6</v>
       </c>
+      <c r="K12">
+        <v>4</v>
+      </c>
       <c r="L12" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="M12" s="6">
         <v>42505</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>4</v>
       </c>
@@ -1893,31 +2055,34 @@
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="E13" t="s">
         <v>9</v>
       </c>
       <c r="F13" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="G13" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="H13" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="I13">
         <v>2</v>
       </c>
+      <c r="K13">
+        <v>4</v>
+      </c>
       <c r="L13" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="M13" s="6">
         <v>42512</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>4</v>
       </c>
@@ -1925,37 +2090,342 @@
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="E14" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="F14" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="G14" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="H14" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="I14">
         <v>6</v>
       </c>
+      <c r="K14">
+        <v>2</v>
+      </c>
       <c r="L14" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="M14" s="6">
         <v>42512</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>98</v>
+      <c r="A15">
+        <v>3</v>
+      </c>
+      <c r="B15">
+        <v>2</v>
+      </c>
+      <c r="C15" t="s">
+        <v>117</v>
+      </c>
+      <c r="E15" t="s">
+        <v>90</v>
+      </c>
+      <c r="F15" t="s">
+        <v>71</v>
+      </c>
+      <c r="H15" t="s">
+        <v>68</v>
       </c>
       <c r="I15">
+        <v>4</v>
+      </c>
+      <c r="L15" t="s">
+        <v>140</v>
+      </c>
+      <c r="M15" s="6">
+        <v>42519</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>3</v>
+      </c>
+      <c r="B16">
+        <v>2</v>
+      </c>
+      <c r="C16" t="s">
+        <v>143</v>
+      </c>
+      <c r="D16" t="s">
+        <v>133</v>
+      </c>
+      <c r="E16" t="s">
+        <v>90</v>
+      </c>
+      <c r="F16" t="s">
+        <v>105</v>
+      </c>
+      <c r="H16" t="s">
+        <v>68</v>
+      </c>
+      <c r="I16">
+        <v>6</v>
+      </c>
+      <c r="L16" t="s">
+        <v>140</v>
+      </c>
+      <c r="M16" s="6">
+        <v>42519</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>3</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17" t="s">
+        <v>121</v>
+      </c>
+      <c r="D17" t="s">
+        <v>134</v>
+      </c>
+      <c r="E17" t="s">
+        <v>58</v>
+      </c>
+      <c r="F17" t="s">
+        <v>93</v>
+      </c>
+      <c r="H17" t="s">
+        <v>68</v>
+      </c>
+      <c r="I17">
+        <v>6</v>
+      </c>
+      <c r="L17" t="s">
+        <v>140</v>
+      </c>
+      <c r="M17" s="6">
+        <v>42519</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>2</v>
+      </c>
+      <c r="B18">
+        <v>2</v>
+      </c>
+      <c r="C18" t="s">
+        <v>118</v>
+      </c>
+      <c r="D18" t="s">
+        <v>142</v>
+      </c>
+      <c r="E18" t="s">
+        <v>58</v>
+      </c>
+      <c r="F18" t="s">
+        <v>110</v>
+      </c>
+      <c r="H18" t="s">
+        <v>68</v>
+      </c>
+      <c r="I18">
+        <v>4</v>
+      </c>
+      <c r="L18" t="s">
+        <v>140</v>
+      </c>
+      <c r="M18" s="6">
+        <v>42519</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>2</v>
+      </c>
+      <c r="B19">
+        <v>2</v>
+      </c>
+      <c r="C19" t="s">
+        <v>119</v>
+      </c>
+      <c r="E19" t="s">
+        <v>59</v>
+      </c>
+      <c r="F19" t="s">
+        <v>110</v>
+      </c>
+      <c r="H19" t="s">
+        <v>68</v>
+      </c>
+      <c r="I19">
+        <v>5</v>
+      </c>
+      <c r="L19" t="s">
+        <v>140</v>
+      </c>
+      <c r="M19" s="6">
+        <v>42519</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>2</v>
+      </c>
+      <c r="B20">
+        <v>2</v>
+      </c>
+      <c r="C20" t="s">
+        <v>120</v>
+      </c>
+      <c r="E20" t="s">
+        <v>90</v>
+      </c>
+      <c r="F20" t="s">
+        <v>93</v>
+      </c>
+      <c r="H20" t="s">
+        <v>68</v>
+      </c>
+      <c r="I20">
+        <v>3</v>
+      </c>
+      <c r="L20" t="s">
+        <v>140</v>
+      </c>
+      <c r="M20" s="6">
+        <v>42519</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>15</v>
+      </c>
+      <c r="B21">
+        <v>2</v>
+      </c>
+      <c r="C21" t="s">
+        <v>122</v>
+      </c>
+      <c r="E21" t="s">
+        <v>58</v>
+      </c>
+      <c r="F21" t="s">
+        <v>91</v>
+      </c>
+      <c r="H21" t="s">
+        <v>68</v>
+      </c>
+      <c r="I21">
+        <v>6</v>
+      </c>
+      <c r="L21" t="s">
+        <v>140</v>
+      </c>
+      <c r="M21" s="6">
+        <v>42519</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>17</v>
+      </c>
+      <c r="B22">
+        <v>2</v>
+      </c>
+      <c r="C22" t="s">
+        <v>137</v>
+      </c>
+      <c r="E22" t="s">
+        <v>58</v>
+      </c>
+      <c r="F22" t="s">
+        <v>138</v>
+      </c>
+      <c r="H22" t="s">
+        <v>67</v>
+      </c>
+      <c r="I22">
+        <v>10</v>
+      </c>
+      <c r="L22" t="s">
+        <v>140</v>
+      </c>
+      <c r="M22" s="6">
+        <v>42519</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>17</v>
+      </c>
+      <c r="B23">
+        <v>2</v>
+      </c>
+      <c r="C23" t="s">
+        <v>135</v>
+      </c>
+      <c r="E23" t="s">
+        <v>136</v>
+      </c>
+      <c r="F23" t="s">
+        <v>103</v>
+      </c>
+      <c r="H23" t="s">
+        <v>67</v>
+      </c>
+      <c r="I23">
+        <v>10</v>
+      </c>
+      <c r="L23" t="s">
+        <v>140</v>
+      </c>
+      <c r="M23" s="6">
+        <v>42519</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>16</v>
+      </c>
+      <c r="B24">
+        <v>2</v>
+      </c>
+      <c r="C24" t="s">
+        <v>124</v>
+      </c>
+      <c r="D24" t="s">
+        <v>125</v>
+      </c>
+      <c r="E24" t="s">
+        <v>90</v>
+      </c>
+      <c r="F24" t="s">
+        <v>138</v>
+      </c>
+      <c r="H24" t="s">
+        <v>67</v>
+      </c>
+      <c r="I24">
+        <v>4</v>
+      </c>
+      <c r="L24" t="s">
+        <v>140</v>
+      </c>
+      <c r="M24" s="6">
+        <v>42519</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>94</v>
+      </c>
+      <c r="I25">
         <f>SUBTOTAL(109,Tabelle1[Planned effort])</f>
-        <v>52</v>
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -1974,14 +2444,14 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.7109375" customWidth="1"/>
-    <col min="4" max="4" width="14.28515625" customWidth="1"/>
+    <col min="2" max="2" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="5" customFormat="1" ht="26.85" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" s="5" customFormat="1" ht="26.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="5" t="s">
         <v>13</v>
       </c>

</xml_diff>

<commit_message>
sprint 2 review, sprint planning 3
</commit_message>
<xml_diff>
--- a/doc/_scrum/scrum_team_yellow.xlsx
+++ b/doc/_scrum/scrum_team_yellow.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14580" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14640" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectTeam" sheetId="3" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="BurndownChart" sheetId="4" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Product Backlog'!$A$1:$H$16</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Product Backlog'!$A$1:$H$20</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Sprint Backlog'!$A$1:$M$1</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="172">
   <si>
     <t>ID</t>
   </si>
@@ -141,21 +141,9 @@
     <t>Printing functionality</t>
   </si>
   <si>
-    <t>Create wiki entries</t>
-  </si>
-  <si>
-    <t>Show wiki entries</t>
-  </si>
-  <si>
     <t>Connect external systems</t>
   </si>
   <si>
-    <t>Create a new wiki article</t>
-  </si>
-  <si>
-    <t>Show wiki article attached to an illness</t>
-  </si>
-  <si>
     <t>Edit a prescription</t>
   </si>
   <si>
@@ -172,9 +160,6 @@
   </si>
   <si>
     <t>Ability to print views</t>
-  </si>
-  <si>
-    <t>Connect medication DB and illness DB</t>
   </si>
   <si>
     <t>Patient overview - base data</t>
@@ -354,9 +339,6 @@
     <t>kevin</t>
   </si>
   <si>
-    <t>in progress</t>
-  </si>
-  <si>
     <t>simon</t>
   </si>
   <si>
@@ -429,15 +411,9 @@
     <t>Improve look &amp; feel of UI (customer feedback)</t>
   </si>
   <si>
-    <t>Task 12</t>
-  </si>
-  <si>
     <t>Adapt UML diagram according to code</t>
   </si>
   <si>
-    <t>Task 13</t>
-  </si>
-  <si>
     <t>Introduce state pattern</t>
   </si>
   <si>
@@ -462,16 +438,124 @@
     <t>Improve usability &amp; menu</t>
   </si>
   <si>
+    <t>Allow to search for patients</t>
+  </si>
+  <si>
+    <t>Connect with patient overview</t>
+  </si>
+  <si>
+    <t>Read real patient data from database</t>
+  </si>
+  <si>
+    <t>Goldplatting</t>
+  </si>
+  <si>
+    <t>Goldplatting optional</t>
+  </si>
+  <si>
+    <t>medikamentensuche, eine person ausgewählt-&gt;navigation ergibt wieder sinn</t>
+  </si>
+  <si>
+    <t>Connect medication DB and illness DB, icd-10 anbinden</t>
+  </si>
+  <si>
+    <t>icons personsearch, link person-&gt;meeting, personsearch results format, personview dropdown weg, navigation person-&gt;doctor (inkl. Der meetings), mainlayout abstand der tiles grösser, annotion meeting notes mehr zeichen, aktuelle prescriptions auf patientenview, patientenview redesign (schmaler), annulieren persrciption</t>
+  </si>
+  <si>
+    <t>Diagnosis for Patient</t>
+  </si>
+  <si>
+    <t>Patient in Session speichern</t>
+  </si>
+  <si>
+    <t>Der User kann einen Patienten auswählen. Dessen Infos werden dann in Person/Prescription/meeting angezeigt</t>
+  </si>
+  <si>
+    <t>Task 12 - UML Domain Model</t>
+  </si>
+  <si>
+    <t>Task 13 - State Pattern</t>
+  </si>
+  <si>
+    <t>simon, alex</t>
+  </si>
+  <si>
+    <t>Code Inspection</t>
+  </si>
+  <si>
+    <t>Diagnosis(illness, date, note)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Patient in Session </t>
+  </si>
+  <si>
+    <t>Diagnosis for patient - model</t>
+  </si>
+  <si>
+    <t>Diagnosis for patient - controller</t>
+  </si>
+  <si>
+    <t>Diagnosis for patient - view</t>
+  </si>
+  <si>
+    <t>Connect or mock illness DB</t>
+  </si>
+  <si>
+    <t>Escalation - button, Patient changes state</t>
+  </si>
+  <si>
+    <t>Escalation - send mail to VGJ1</t>
+  </si>
+  <si>
+    <t>Show illnesses in GUI</t>
+  </si>
+  <si>
+    <t>Create illness model</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Controller </t>
+  </si>
+  <si>
+    <t>Link meeting tile to meeting details</t>
+  </si>
+  <si>
+    <t>Insert Grid Layout</t>
+  </si>
+  <si>
+    <t>Rework person search view</t>
+  </si>
+  <si>
+    <t>FindBugs incl. Corrections</t>
+  </si>
+  <si>
+    <t>incl. search for illnesses</t>
+  </si>
+  <si>
+    <t>mock it first</t>
+  </si>
+  <si>
+    <t>incl. adaption of menu</t>
+  </si>
+  <si>
+    <t>date of diagnosis, illness-id, (notes)</t>
+  </si>
+  <si>
+    <t>icd-10 style</t>
+  </si>
+  <si>
+    <t>Button in wiki, adapt person view, popup to enter notes after clicking button</t>
+  </si>
+  <si>
+    <t>Dropdown in GUI, enum on DB</t>
+  </si>
+  <si>
+    <t>domi, simon</t>
+  </si>
+  <si>
+    <t>Insert icons, shadows, margins</t>
+  </si>
+  <si>
     <t>assigned</t>
-  </si>
-  <si>
-    <t>Allow to search for patients</t>
-  </si>
-  <si>
-    <t>Connect with patient overview</t>
-  </si>
-  <si>
-    <t>Read real patient data from database</t>
   </si>
 </sst>
 </file>
@@ -556,14 +640,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -588,12 +674,21 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="7">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Stand." xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
@@ -638,11 +733,11 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A1:M25" totalsRowCount="1" headerRowDxfId="1">
-  <autoFilter ref="A1:M24">
-    <filterColumn colId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A1:M38" totalsRowCount="1" headerRowDxfId="1">
+  <autoFilter ref="A1:M37">
+    <filterColumn colId="11">
       <filters>
-        <filter val="2"/>
+        <filter val="assigned"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -957,7 +1052,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="148" zoomScaleNormal="148" zoomScalePageLayoutView="148" workbookViewId="0">
+    <sheetView zoomScale="148" zoomScaleNormal="148" zoomScalePageLayoutView="148" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -976,7 +1071,7 @@
         <v>12</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -987,7 +1082,7 @@
         <v>28</v>
       </c>
       <c r="C2" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -998,7 +1093,7 @@
         <v>26</v>
       </c>
       <c r="C3" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -1009,7 +1104,7 @@
         <v>25</v>
       </c>
       <c r="C4" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -1020,7 +1115,7 @@
         <v>27</v>
       </c>
       <c r="C5" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -1031,7 +1126,7 @@
         <v>24</v>
       </c>
       <c r="C6" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -1042,55 +1137,55 @@
         <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="7" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B10" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="B13" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>
@@ -1100,17 +1195,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I18"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView zoomScale="142" zoomScaleNormal="142" zoomScalePageLayoutView="142" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3.6640625" customWidth="1"/>
     <col min="2" max="2" width="37.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42.5" customWidth="1"/>
+    <col min="3" max="3" width="92.6640625" customWidth="1"/>
     <col min="4" max="4" width="18.83203125" customWidth="1"/>
     <col min="5" max="5" width="11.6640625" customWidth="1"/>
     <col min="6" max="6" width="13.1640625" customWidth="1"/>
@@ -1130,13 +1225,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>10</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>8</v>
@@ -1145,7 +1240,7 @@
         <v>4</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -1153,7 +1248,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>29</v>
@@ -1171,10 +1266,10 @@
         <v>16</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -1182,10 +1277,10 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="C3" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D3" s="1">
         <v>998</v>
@@ -1200,10 +1295,10 @@
         <v>16</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="I3" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -1211,10 +1306,10 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C4" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="D4" s="1">
         <v>997</v>
@@ -1229,10 +1324,10 @@
         <v>16</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="I4" t="s">
-        <v>111</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -1240,10 +1335,10 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>109</v>
+        <v>103</v>
       </c>
       <c r="C5" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="D5" s="1">
         <v>996</v>
@@ -1258,10 +1353,10 @@
         <v>0</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>104</v>
+        <v>110</v>
       </c>
       <c r="I5" t="s">
-        <v>112</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -1269,10 +1364,10 @@
         <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>129</v>
+        <v>143</v>
       </c>
       <c r="C6" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="D6" s="1">
         <v>995</v>
@@ -1287,10 +1382,10 @@
         <v>0</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>51</v>
+        <v>110</v>
       </c>
       <c r="I6" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -1298,10 +1393,10 @@
         <v>17</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>131</v>
+        <v>144</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="D7" s="1">
         <v>994</v>
@@ -1316,7 +1411,7 @@
         <v>0</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>51</v>
+        <v>110</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -1327,7 +1422,7 @@
         <v>30</v>
       </c>
       <c r="C8" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="D8" s="1">
         <v>993</v>
@@ -1342,7 +1437,7 @@
         <v>0</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>51</v>
+        <v>110</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -1350,16 +1445,16 @@
         <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
       <c r="C9" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="D9" s="1">
         <v>992</v>
       </c>
       <c r="E9">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="F9" s="1">
         <v>0</v>
@@ -1368,7 +1463,7 @@
         <v>0</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>51</v>
+        <v>110</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -1376,10 +1471,10 @@
         <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
       <c r="C10" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="D10" s="1">
         <v>991</v>
@@ -1394,21 +1489,21 @@
         <v>0</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>51</v>
+        <v>110</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="1">
-        <v>5</v>
+      <c r="A11">
+        <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>35</v>
+        <v>135</v>
       </c>
       <c r="C11" t="s">
-        <v>38</v>
+        <v>139</v>
       </c>
       <c r="D11" s="1">
-        <v>1</v>
+        <v>990</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -1420,21 +1515,21 @@
         <v>0</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C12" t="s">
-        <v>39</v>
+        <v>138</v>
       </c>
       <c r="D12" s="1">
-        <v>1</v>
+        <v>989</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -1446,21 +1541,21 @@
         <v>0</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="B13" t="s">
-        <v>108</v>
+        <v>141</v>
       </c>
       <c r="C13" t="s">
-        <v>40</v>
-      </c>
-      <c r="D13" s="1">
-        <v>1</v>
+        <v>142</v>
+      </c>
+      <c r="D13" s="10">
+        <v>989</v>
       </c>
       <c r="E13">
         <v>0</v>
@@ -1472,47 +1567,47 @@
         <v>0</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="1">
+      <c r="A14">
+        <v>20</v>
+      </c>
+      <c r="B14" t="s">
+        <v>140</v>
+      </c>
+      <c r="C14" t="s">
+        <v>147</v>
+      </c>
+      <c r="D14" s="1">
+        <v>986</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14" s="1">
+        <v>0</v>
+      </c>
+      <c r="G14" s="1">
+        <v>0</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
         <v>9</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B15" t="s">
         <v>31</v>
       </c>
-      <c r="C14" t="s">
-        <v>42</v>
-      </c>
-      <c r="D14" s="1">
-        <v>1</v>
-      </c>
-      <c r="E14">
-        <v>0</v>
-      </c>
-      <c r="F14" s="1">
-        <v>0</v>
-      </c>
-      <c r="G14" s="1">
-        <v>0</v>
-      </c>
-      <c r="H14" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>10</v>
-      </c>
-      <c r="B15" t="s">
-        <v>32</v>
-      </c>
       <c r="C15" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="D15" s="1">
-        <v>1</v>
+        <v>985</v>
       </c>
       <c r="E15">
         <v>0</v>
@@ -1524,7 +1619,7 @@
         <v>0</v>
       </c>
       <c r="H15" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
@@ -1535,10 +1630,10 @@
         <v>33</v>
       </c>
       <c r="C16" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D16" s="1">
-        <v>1</v>
+        <v>500</v>
       </c>
       <c r="E16">
         <v>0</v>
@@ -1550,65 +1645,117 @@
         <v>0</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A17" s="1">
+      <c r="A17">
+        <v>19</v>
+      </c>
+      <c r="B17" t="s">
+        <v>136</v>
+      </c>
+      <c r="C17" t="s">
+        <v>137</v>
+      </c>
+      <c r="D17" s="1">
+        <v>980</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17" s="1">
+        <v>0</v>
+      </c>
+      <c r="G17" s="1">
+        <v>0</v>
+      </c>
+      <c r="H17" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>7</v>
+      </c>
+      <c r="B18" t="s">
+        <v>102</v>
+      </c>
+      <c r="C18" t="s">
+        <v>36</v>
+      </c>
+      <c r="D18" s="1">
+        <v>500</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18" s="1">
+        <v>0</v>
+      </c>
+      <c r="G18" s="1">
+        <v>0</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>10</v>
+      </c>
+      <c r="B19" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" t="s">
+        <v>39</v>
+      </c>
+      <c r="D19" s="1">
+        <v>500</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19" s="1">
+        <v>0</v>
+      </c>
+      <c r="G19" s="1">
+        <v>0</v>
+      </c>
+      <c r="H19" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" s="11">
         <v>13</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B20" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="C17" t="s">
-        <v>45</v>
-      </c>
-      <c r="D17" s="1">
-        <v>1</v>
-      </c>
-      <c r="E17">
-        <v>0</v>
-      </c>
-      <c r="F17" s="1">
-        <v>0</v>
-      </c>
-      <c r="G17" s="1">
-        <v>0</v>
-      </c>
-      <c r="H17" s="1" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>14</v>
-      </c>
-      <c r="B18" t="s">
-        <v>37</v>
-      </c>
-      <c r="C18" t="s">
+      <c r="C20" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" s="11">
+        <v>500</v>
+      </c>
+      <c r="E20" s="12">
+        <v>0</v>
+      </c>
+      <c r="F20" s="11">
+        <v>0</v>
+      </c>
+      <c r="G20" s="11">
+        <v>0</v>
+      </c>
+      <c r="H20" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="D18" s="1">
-        <v>1</v>
-      </c>
-      <c r="E18">
-        <v>0</v>
-      </c>
-      <c r="F18" s="1">
-        <v>0</v>
-      </c>
-      <c r="G18" s="1">
-        <v>0</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>51</v>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H16">
-    <sortState ref="A2:H18">
-      <sortCondition descending="1" ref="D1:D18"/>
+  <autoFilter ref="A1:H20">
+    <sortState ref="A2:H22">
+      <sortCondition descending="1" ref="D1:D22"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1618,18 +1765,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M25"/>
+  <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="139" zoomScaleNormal="139" zoomScalePageLayoutView="139" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L37" sqref="L37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.1640625" customWidth="1"/>
-    <col min="3" max="3" width="32.1640625" customWidth="1"/>
-    <col min="4" max="4" width="24" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="38.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.33203125" customWidth="1"/>
     <col min="5" max="5" width="15.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.6640625" customWidth="1"/>
@@ -1637,13 +1784,13 @@
     <col min="9" max="9" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17.6640625" hidden="1" customWidth="1"/>
     <col min="11" max="11" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="39.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.33203125" customWidth="1"/>
     <col min="13" max="13" width="11.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="4" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>6</v>
@@ -1652,13 +1799,13 @@
         <v>1</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>7</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>11</v>
@@ -1667,19 +1814,19 @@
         <v>3</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="L1" s="9" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
@@ -1690,28 +1837,28 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="D2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E2" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="F2" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="G2" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="H2" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="I2">
         <v>8</v>
       </c>
       <c r="L2" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="M2" s="6">
         <v>42504</v>
@@ -1725,22 +1872,22 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="D3" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="E3" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="F3" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="G3" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
       <c r="H3" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="I3">
         <v>8</v>
@@ -1749,7 +1896,7 @@
         <v>4</v>
       </c>
       <c r="L3" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="M3" s="6">
         <v>42504</v>
@@ -1763,25 +1910,25 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E4" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="F4" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="G4" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="H4" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="I4">
         <v>6</v>
       </c>
       <c r="L4" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="M4" s="6">
         <v>42505</v>
@@ -1795,26 +1942,26 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" t="s">
         <v>9</v>
       </c>
       <c r="F5" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="G5" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="H5" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="I5">
         <v>2</v>
       </c>
       <c r="L5" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="M5" s="6">
         <v>42512</v>
@@ -1828,25 +1975,25 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="E6" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="F6" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="G6" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="H6" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="I6">
         <v>6</v>
       </c>
       <c r="L6" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="M6" s="6">
         <v>42512</v>
@@ -1860,25 +2007,25 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="E7" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="F7" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="G7" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="H7" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="I7">
         <v>2</v>
       </c>
       <c r="L7" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="M7" s="6">
         <v>42512</v>
@@ -1892,25 +2039,25 @@
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="E8" t="s">
         <v>9</v>
       </c>
       <c r="F8" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="G8" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="H8" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="I8">
         <v>1</v>
       </c>
       <c r="L8" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="M8" s="6">
         <v>42512</v>
@@ -1924,25 +2071,25 @@
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="E9" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="F9" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="G9" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="H9" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="I9">
         <v>1</v>
       </c>
       <c r="L9" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="M9" s="6">
         <v>42512</v>
@@ -1956,25 +2103,25 @@
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="E10" t="s">
         <v>9</v>
       </c>
       <c r="F10" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="G10" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="H10" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="I10">
         <v>2</v>
       </c>
       <c r="L10" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="M10" s="6">
         <v>42512</v>
@@ -1988,25 +2135,25 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="E11" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="F11" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="G11" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="H11" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="I11">
         <v>2</v>
       </c>
       <c r="L11" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="M11" s="6">
         <v>42505</v>
@@ -2020,19 +2167,19 @@
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="E12" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="F12" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="G12" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="H12" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="I12">
         <v>6</v>
@@ -2041,7 +2188,7 @@
         <v>4</v>
       </c>
       <c r="L12" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="M12" s="6">
         <v>42505</v>
@@ -2055,19 +2202,19 @@
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E13" t="s">
         <v>9</v>
       </c>
       <c r="F13" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="G13" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="H13" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="I13">
         <v>2</v>
@@ -2076,7 +2223,7 @@
         <v>4</v>
       </c>
       <c r="L13" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="M13" s="6">
         <v>42512</v>
@@ -2090,19 +2237,19 @@
         <v>1</v>
       </c>
       <c r="C14" t="s">
+        <v>49</v>
+      </c>
+      <c r="E14" t="s">
         <v>54</v>
       </c>
-      <c r="E14" t="s">
-        <v>59</v>
-      </c>
       <c r="F14" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="G14" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="H14" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="I14">
         <v>6</v>
@@ -2111,13 +2258,13 @@
         <v>2</v>
       </c>
       <c r="L14" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="M14" s="6">
         <v>42512</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>3</v>
       </c>
@@ -2125,28 +2272,31 @@
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="E15" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="F15" t="s">
-        <v>71</v>
+        <v>66</v>
+      </c>
+      <c r="G15" t="s">
+        <v>98</v>
       </c>
       <c r="H15" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="I15">
         <v>4</v>
       </c>
       <c r="L15" t="s">
-        <v>140</v>
+        <v>110</v>
       </c>
       <c r="M15" s="6">
         <v>42519</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>3</v>
       </c>
@@ -2154,31 +2304,34 @@
         <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="D16" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="E16" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="F16" t="s">
-        <v>105</v>
+        <v>99</v>
+      </c>
+      <c r="G16" t="s">
+        <v>66</v>
       </c>
       <c r="H16" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="I16">
         <v>6</v>
       </c>
       <c r="L16" t="s">
-        <v>140</v>
+        <v>110</v>
       </c>
       <c r="M16" s="6">
         <v>42519</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>3</v>
       </c>
@@ -2186,31 +2339,34 @@
         <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="D17" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="E17" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="F17" t="s">
-        <v>93</v>
+        <v>88</v>
+      </c>
+      <c r="G17" t="s">
+        <v>104</v>
       </c>
       <c r="H17" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="I17">
         <v>6</v>
       </c>
       <c r="L17" t="s">
-        <v>140</v>
+        <v>110</v>
       </c>
       <c r="M17" s="6">
         <v>42519</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>2</v>
       </c>
@@ -2218,31 +2374,34 @@
         <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="D18" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="E18" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="F18" t="s">
-        <v>110</v>
+        <v>104</v>
+      </c>
+      <c r="G18" t="s">
+        <v>88</v>
       </c>
       <c r="H18" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="I18">
         <v>4</v>
       </c>
       <c r="L18" t="s">
-        <v>140</v>
+        <v>110</v>
       </c>
       <c r="M18" s="6">
         <v>42519</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>2</v>
       </c>
@@ -2250,28 +2409,31 @@
         <v>2</v>
       </c>
       <c r="C19" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="E19" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="F19" t="s">
-        <v>110</v>
+        <v>104</v>
+      </c>
+      <c r="G19" t="s">
+        <v>88</v>
       </c>
       <c r="H19" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="I19">
         <v>5</v>
       </c>
       <c r="L19" t="s">
-        <v>140</v>
+        <v>110</v>
       </c>
       <c r="M19" s="6">
         <v>42519</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>2</v>
       </c>
@@ -2279,28 +2441,31 @@
         <v>2</v>
       </c>
       <c r="C20" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="E20" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="F20" t="s">
-        <v>93</v>
+        <v>88</v>
+      </c>
+      <c r="G20" t="s">
+        <v>104</v>
       </c>
       <c r="H20" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="I20">
         <v>3</v>
       </c>
       <c r="L20" t="s">
-        <v>140</v>
+        <v>110</v>
       </c>
       <c r="M20" s="6">
         <v>42519</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>15</v>
       </c>
@@ -2308,28 +2473,31 @@
         <v>2</v>
       </c>
       <c r="C21" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="E21" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="F21" t="s">
-        <v>91</v>
+        <v>86</v>
+      </c>
+      <c r="G21" t="s">
+        <v>100</v>
       </c>
       <c r="H21" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="I21">
         <v>6</v>
       </c>
       <c r="L21" t="s">
-        <v>140</v>
+        <v>110</v>
       </c>
       <c r="M21" s="6">
         <v>42519</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>17</v>
       </c>
@@ -2337,28 +2505,31 @@
         <v>2</v>
       </c>
       <c r="C22" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="E22" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="F22" t="s">
-        <v>138</v>
+        <v>130</v>
+      </c>
+      <c r="G22" t="s">
+        <v>98</v>
       </c>
       <c r="H22" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="I22">
         <v>10</v>
       </c>
       <c r="L22" t="s">
-        <v>140</v>
+        <v>110</v>
       </c>
       <c r="M22" s="6">
         <v>42519</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>17</v>
       </c>
@@ -2366,28 +2537,31 @@
         <v>2</v>
       </c>
       <c r="C23" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="E23" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="F23" t="s">
-        <v>103</v>
+        <v>98</v>
+      </c>
+      <c r="G23" t="s">
+        <v>145</v>
       </c>
       <c r="H23" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="I23">
         <v>10</v>
       </c>
       <c r="L23" t="s">
-        <v>140</v>
+        <v>110</v>
       </c>
       <c r="M23" s="6">
         <v>42519</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>16</v>
       </c>
@@ -2395,37 +2569,450 @@
         <v>2</v>
       </c>
       <c r="C24" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
       <c r="D24" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="E24" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="F24" t="s">
-        <v>138</v>
+        <v>130</v>
+      </c>
+      <c r="G24" t="s">
+        <v>100</v>
       </c>
       <c r="H24" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="I24">
         <v>4</v>
       </c>
       <c r="L24" t="s">
-        <v>140</v>
+        <v>110</v>
       </c>
       <c r="M24" s="6">
         <v>42519</v>
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>94</v>
+      <c r="A25">
+        <v>18</v>
+      </c>
+      <c r="B25">
+        <v>3</v>
+      </c>
+      <c r="C25" t="s">
+        <v>146</v>
+      </c>
+      <c r="D25" t="s">
+        <v>161</v>
+      </c>
+      <c r="E25" t="s">
+        <v>100</v>
+      </c>
+      <c r="F25" t="s">
+        <v>66</v>
+      </c>
+      <c r="H25" t="s">
+        <v>62</v>
       </c>
       <c r="I25">
+        <v>3</v>
+      </c>
+      <c r="K25">
+        <v>0</v>
+      </c>
+      <c r="L25" t="s">
+        <v>171</v>
+      </c>
+      <c r="M25" s="6">
+        <v>42535</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>14</v>
+      </c>
+      <c r="B26">
+        <v>3</v>
+      </c>
+      <c r="C26" t="s">
+        <v>156</v>
+      </c>
+      <c r="D26" t="s">
+        <v>166</v>
+      </c>
+      <c r="E26" t="s">
+        <v>85</v>
+      </c>
+      <c r="F26" t="s">
+        <v>98</v>
+      </c>
+      <c r="H26" t="s">
+        <v>63</v>
+      </c>
+      <c r="I26">
+        <v>6</v>
+      </c>
+      <c r="L26" t="s">
+        <v>171</v>
+      </c>
+      <c r="M26" s="6">
+        <v>42535</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>14</v>
+      </c>
+      <c r="B27">
+        <v>3</v>
+      </c>
+      <c r="C27" t="s">
+        <v>155</v>
+      </c>
+      <c r="D27" t="s">
+        <v>162</v>
+      </c>
+      <c r="E27" t="s">
+        <v>53</v>
+      </c>
+      <c r="F27" t="s">
+        <v>88</v>
+      </c>
+      <c r="H27" t="s">
+        <v>63</v>
+      </c>
+      <c r="I27">
+        <v>6</v>
+      </c>
+      <c r="L27" t="s">
+        <v>171</v>
+      </c>
+      <c r="M27" s="6">
+        <v>42535</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>14</v>
+      </c>
+      <c r="B28">
+        <v>3</v>
+      </c>
+      <c r="C28" t="s">
+        <v>152</v>
+      </c>
+      <c r="D28" t="s">
+        <v>163</v>
+      </c>
+      <c r="E28" t="s">
+        <v>157</v>
+      </c>
+      <c r="F28" t="s">
+        <v>98</v>
+      </c>
+      <c r="H28" t="s">
+        <v>63</v>
+      </c>
+      <c r="I28">
+        <v>14</v>
+      </c>
+      <c r="L28" t="s">
+        <v>171</v>
+      </c>
+      <c r="M28" s="6">
+        <v>42535</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>21</v>
+      </c>
+      <c r="B29">
+        <v>3</v>
+      </c>
+      <c r="C29" t="s">
+        <v>148</v>
+      </c>
+      <c r="D29" t="s">
+        <v>164</v>
+      </c>
+      <c r="E29" t="s">
+        <v>100</v>
+      </c>
+      <c r="F29" t="s">
+        <v>99</v>
+      </c>
+      <c r="H29" t="s">
+        <v>62</v>
+      </c>
+      <c r="I29">
+        <v>10</v>
+      </c>
+      <c r="K29">
+        <v>0</v>
+      </c>
+      <c r="L29" t="s">
+        <v>171</v>
+      </c>
+      <c r="M29" s="6">
+        <v>42535</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>20</v>
+      </c>
+      <c r="B30">
+        <v>3</v>
+      </c>
+      <c r="C30" t="s">
+        <v>149</v>
+      </c>
+      <c r="D30" t="s">
+        <v>165</v>
+      </c>
+      <c r="E30" t="s">
+        <v>85</v>
+      </c>
+      <c r="F30" t="s">
+        <v>66</v>
+      </c>
+      <c r="H30" t="s">
+        <v>63</v>
+      </c>
+      <c r="I30">
+        <v>4</v>
+      </c>
+      <c r="L30" t="s">
+        <v>171</v>
+      </c>
+      <c r="M30" s="6">
+        <v>42535</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>20</v>
+      </c>
+      <c r="B31">
+        <v>3</v>
+      </c>
+      <c r="C31" t="s">
+        <v>150</v>
+      </c>
+      <c r="E31" t="s">
+        <v>54</v>
+      </c>
+      <c r="F31" t="s">
+        <v>66</v>
+      </c>
+      <c r="H31" t="s">
+        <v>63</v>
+      </c>
+      <c r="I31">
+        <v>4</v>
+      </c>
+      <c r="L31" t="s">
+        <v>171</v>
+      </c>
+      <c r="M31" s="6">
+        <v>42535</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>20</v>
+      </c>
+      <c r="B32">
+        <v>3</v>
+      </c>
+      <c r="C32" t="s">
+        <v>151</v>
+      </c>
+      <c r="D32" t="s">
+        <v>167</v>
+      </c>
+      <c r="E32" t="s">
+        <v>53</v>
+      </c>
+      <c r="F32" t="s">
+        <v>104</v>
+      </c>
+      <c r="H32" t="s">
+        <v>63</v>
+      </c>
+      <c r="I32">
+        <v>6</v>
+      </c>
+      <c r="L32" t="s">
+        <v>171</v>
+      </c>
+      <c r="M32" s="6">
+        <v>42535</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>9</v>
+      </c>
+      <c r="B33">
+        <v>3</v>
+      </c>
+      <c r="C33" t="s">
+        <v>153</v>
+      </c>
+      <c r="D33" t="s">
+        <v>168</v>
+      </c>
+      <c r="E33" t="s">
+        <v>53</v>
+      </c>
+      <c r="F33" t="s">
+        <v>86</v>
+      </c>
+      <c r="H33" t="s">
+        <v>63</v>
+      </c>
+      <c r="I33">
+        <v>6</v>
+      </c>
+      <c r="L33" t="s">
+        <v>171</v>
+      </c>
+      <c r="M33" s="6">
+        <v>42535</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>9</v>
+      </c>
+      <c r="B34">
+        <v>3</v>
+      </c>
+      <c r="C34" t="s">
+        <v>154</v>
+      </c>
+      <c r="E34" t="s">
+        <v>54</v>
+      </c>
+      <c r="F34" t="s">
+        <v>169</v>
+      </c>
+      <c r="H34" t="s">
+        <v>63</v>
+      </c>
+      <c r="I34">
+        <v>8</v>
+      </c>
+      <c r="L34" t="s">
+        <v>171</v>
+      </c>
+      <c r="M34" s="6">
+        <v>42535</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>18</v>
+      </c>
+      <c r="B35">
+        <v>3</v>
+      </c>
+      <c r="C35" t="s">
+        <v>160</v>
+      </c>
+      <c r="D35" t="s">
+        <v>159</v>
+      </c>
+      <c r="E35" t="s">
+        <v>53</v>
+      </c>
+      <c r="F35" t="s">
+        <v>104</v>
+      </c>
+      <c r="H35" t="s">
+        <v>63</v>
+      </c>
+      <c r="I35">
+        <v>2</v>
+      </c>
+      <c r="L35" t="s">
+        <v>110</v>
+      </c>
+      <c r="M35" s="6">
+        <v>42535</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>18</v>
+      </c>
+      <c r="B36">
+        <v>3</v>
+      </c>
+      <c r="C36" t="s">
+        <v>170</v>
+      </c>
+      <c r="E36" t="s">
+        <v>53</v>
+      </c>
+      <c r="F36" t="s">
+        <v>88</v>
+      </c>
+      <c r="H36" t="s">
+        <v>63</v>
+      </c>
+      <c r="I36">
+        <v>3</v>
+      </c>
+      <c r="L36" t="s">
+        <v>171</v>
+      </c>
+      <c r="M36" s="6">
+        <v>42535</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>18</v>
+      </c>
+      <c r="B37">
+        <v>3</v>
+      </c>
+      <c r="C37" t="s">
+        <v>158</v>
+      </c>
+      <c r="E37" t="s">
+        <v>53</v>
+      </c>
+      <c r="F37" t="s">
+        <v>86</v>
+      </c>
+      <c r="H37" t="s">
+        <v>63</v>
+      </c>
+      <c r="I37">
+        <v>2</v>
+      </c>
+      <c r="L37" t="s">
+        <v>110</v>
+      </c>
+      <c r="M37" s="6">
+        <v>42535</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>89</v>
+      </c>
+      <c r="I38">
         <f>SUBTOTAL(109,Tabelle1[Planned effort])</f>
-        <v>58</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -2440,7 +3027,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Final scrum backlog, burndown chart
</commit_message>
<xml_diff>
--- a/doc/_scrum/scrum_team_yellow.xlsx
+++ b/doc/_scrum/scrum_team_yellow.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14640" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14600" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectTeam" sheetId="3" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="168">
   <si>
     <t>ID</t>
   </si>
@@ -73,18 +73,6 @@
   </si>
   <si>
     <t>GitHub Alias</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sprint </t>
-  </si>
-  <si>
-    <t>Remaining Effort</t>
-  </si>
-  <si>
-    <t>Remaining Ressources</t>
-  </si>
-  <si>
-    <t>Time of Record</t>
   </si>
   <si>
     <t>Simon Schaad</t>
@@ -543,9 +531,6 @@
     <t>icd-10 style</t>
   </si>
   <si>
-    <t>Button in wiki, adapt person view, popup to enter notes after clicking button</t>
-  </si>
-  <si>
     <t>Dropdown in GUI, enum on DB</t>
   </si>
   <si>
@@ -555,14 +540,17 @@
     <t>Insert icons, shadows, margins</t>
   </si>
   <si>
-    <t>assigned</t>
+    <t>Button in wiki, show current illness in person view, popup to enter notes after clicking button</t>
+  </si>
+  <si>
+    <t>see separate file</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -610,8 +598,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri (Textkörper)"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -624,19 +618,22 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="3"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -649,7 +646,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
@@ -662,9 +659,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -681,6 +675,18 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
@@ -734,13 +740,7 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabelle1" displayName="Tabelle1" ref="A1:M38" totalsRowCount="1" headerRowDxfId="1">
-  <autoFilter ref="A1:M37">
-    <filterColumn colId="11">
-      <filters>
-        <filter val="assigned"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:M37"/>
   <sortState ref="A2:M14">
     <sortCondition ref="H1:H14"/>
   </sortState>
@@ -1053,13 +1053,13 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView zoomScale="148" zoomScaleNormal="148" zoomScalePageLayoutView="148" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="61.5" customWidth="1"/>
     <col min="3" max="3" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1071,121 +1071,121 @@
         <v>12</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C2" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="C3" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C4" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C5" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="C6" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="B9" s="7" t="s">
-        <v>72</v>
+      <c r="A9" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B9" s="6" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B10" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>67</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>74</v>
+        <v>63</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>69</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>97</v>
+        <v>65</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B13" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="60" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>70</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>93</v>
+        <v>66</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -1198,20 +1198,20 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD11"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3.6640625" customWidth="1"/>
-    <col min="2" max="2" width="37.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="92.6640625" customWidth="1"/>
+    <col min="2" max="2" width="36" customWidth="1"/>
+    <col min="3" max="3" width="31.1640625" customWidth="1"/>
     <col min="4" max="4" width="18.83203125" customWidth="1"/>
     <col min="5" max="5" width="11.6640625" customWidth="1"/>
     <col min="6" max="6" width="13.1640625" customWidth="1"/>
-    <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.5" customWidth="1"/>
-    <col min="9" max="9" width="48.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.6640625" customWidth="1"/>
+    <col min="8" max="8" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="40.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.2">
@@ -1225,13 +1225,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>10</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>8</v>
@@ -1240,7 +1240,7 @@
         <v>4</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -1248,10 +1248,10 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D2" s="1">
         <v>999</v>
@@ -1266,10 +1266,10 @@
         <v>16</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -1277,10 +1277,10 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C3" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="D3" s="1">
         <v>998</v>
@@ -1295,10 +1295,10 @@
         <v>16</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="I3" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -1306,10 +1306,10 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="C4" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D4" s="1">
         <v>997</v>
@@ -1324,10 +1324,10 @@
         <v>16</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="I4" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -1335,10 +1335,10 @@
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C5" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="D5" s="1">
         <v>996</v>
@@ -1353,10 +1353,10 @@
         <v>0</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="I5" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -1364,10 +1364,10 @@
         <v>16</v>
       </c>
       <c r="B6" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C6" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D6" s="1">
         <v>995</v>
@@ -1382,10 +1382,10 @@
         <v>0</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="I6" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -1393,10 +1393,10 @@
         <v>17</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="D7" s="1">
         <v>994</v>
@@ -1411,7 +1411,7 @@
         <v>0</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -1419,10 +1419,10 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C8" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="D8" s="1">
         <v>993</v>
@@ -1437,7 +1437,7 @@
         <v>0</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -1445,10 +1445,10 @@
         <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="C9" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="D9" s="1">
         <v>992</v>
@@ -1463,7 +1463,7 @@
         <v>0</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -1471,10 +1471,10 @@
         <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C10" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D10" s="1">
         <v>991</v>
@@ -1489,7 +1489,7 @@
         <v>0</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
@@ -1497,16 +1497,16 @@
         <v>18</v>
       </c>
       <c r="B11" t="s">
+        <v>131</v>
+      </c>
+      <c r="C11" t="s">
         <v>135</v>
-      </c>
-      <c r="C11" t="s">
-        <v>139</v>
       </c>
       <c r="D11" s="1">
         <v>990</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F11" s="1">
         <v>0</v>
@@ -1515,7 +1515,7 @@
         <v>0</v>
       </c>
       <c r="H11" s="1" t="s">
-        <v>46</v>
+        <v>106</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
@@ -1523,16 +1523,16 @@
         <v>14</v>
       </c>
       <c r="B12" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C12" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="D12" s="1">
         <v>989</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="F12" s="1">
         <v>0</v>
@@ -1541,7 +1541,7 @@
         <v>0</v>
       </c>
       <c r="H12" s="1" t="s">
-        <v>46</v>
+        <v>106</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
@@ -1549,16 +1549,16 @@
         <v>21</v>
       </c>
       <c r="B13" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C13" t="s">
-        <v>142</v>
-      </c>
-      <c r="D13" s="10">
+        <v>138</v>
+      </c>
+      <c r="D13" s="9">
         <v>989</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F13" s="1">
         <v>0</v>
@@ -1567,7 +1567,7 @@
         <v>0</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>46</v>
+        <v>106</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
@@ -1575,16 +1575,16 @@
         <v>20</v>
       </c>
       <c r="B14" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C14" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="D14" s="1">
         <v>986</v>
       </c>
       <c r="E14">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="F14" s="1">
         <v>0</v>
@@ -1593,33 +1593,33 @@
         <v>0</v>
       </c>
       <c r="H14" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="1">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" s="17" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="16">
         <v>9</v>
       </c>
-      <c r="B15" t="s">
-        <v>31</v>
-      </c>
-      <c r="C15" t="s">
-        <v>38</v>
-      </c>
-      <c r="D15" s="1">
+      <c r="B15" s="17" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" s="16">
         <v>985</v>
       </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
-      <c r="F15" s="1">
-        <v>0</v>
-      </c>
-      <c r="G15" s="1">
-        <v>0</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>46</v>
+      <c r="E15" s="17">
+        <v>28</v>
+      </c>
+      <c r="F15" s="16">
+        <v>0</v>
+      </c>
+      <c r="G15" s="16">
+        <v>0</v>
+      </c>
+      <c r="H15" s="16" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
@@ -1627,10 +1627,10 @@
         <v>12</v>
       </c>
       <c r="B16" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C16" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="D16" s="1">
         <v>500</v>
@@ -1645,7 +1645,7 @@
         <v>0</v>
       </c>
       <c r="H16" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
@@ -1653,10 +1653,10 @@
         <v>19</v>
       </c>
       <c r="B17" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C17" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="D17" s="1">
         <v>980</v>
@@ -1671,18 +1671,18 @@
         <v>0</v>
       </c>
       <c r="H17" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" s="12" customFormat="1" x14ac:dyDescent="0.2">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" s="11" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>7</v>
       </c>
       <c r="B18" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="C18" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D18" s="1">
         <v>500</v>
@@ -1697,7 +1697,7 @@
         <v>0</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
@@ -1705,10 +1705,10 @@
         <v>10</v>
       </c>
       <c r="B19" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C19" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="D19" s="1">
         <v>500</v>
@@ -1723,33 +1723,33 @@
         <v>0</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A20" s="11">
+      <c r="A20" s="10">
         <v>13</v>
       </c>
-      <c r="B20" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="C20" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="D20" s="11">
+      <c r="B20" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20" s="10">
         <v>500</v>
       </c>
-      <c r="E20" s="12">
-        <v>0</v>
-      </c>
-      <c r="F20" s="11">
-        <v>0</v>
-      </c>
-      <c r="G20" s="11">
-        <v>0</v>
-      </c>
-      <c r="H20" s="11" t="s">
-        <v>46</v>
+      <c r="E20" s="11">
+        <v>0</v>
+      </c>
+      <c r="F20" s="10">
+        <v>0</v>
+      </c>
+      <c r="G20" s="10">
+        <v>0</v>
+      </c>
+      <c r="H20" s="10" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -1767,8 +1767,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L37" sqref="L37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12:K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1776,7 +1776,7 @@
     <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="6.1640625" customWidth="1"/>
     <col min="3" max="3" width="38.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="32.33203125" customWidth="1"/>
+    <col min="4" max="4" width="49.1640625" customWidth="1"/>
     <col min="5" max="5" width="15.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.83203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="9.6640625" customWidth="1"/>
@@ -1790,7 +1790,7 @@
   <sheetData>
     <row r="1" spans="1:13" s="4" customFormat="1" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>6</v>
@@ -1799,13 +1799,13 @@
         <v>1</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>7</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="G1" s="4" t="s">
         <v>11</v>
@@ -1814,22 +1814,22 @@
         <v>3</v>
       </c>
       <c r="I1" s="4" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="L1" s="9" t="s">
-        <v>90</v>
+        <v>92</v>
+      </c>
+      <c r="L1" s="8" t="s">
+        <v>86</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>11</v>
       </c>
@@ -1837,34 +1837,34 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="D2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2" t="s">
+        <v>73</v>
+      </c>
+      <c r="G2" t="s">
+        <v>62</v>
+      </c>
+      <c r="H2" t="s">
         <v>58</v>
-      </c>
-      <c r="E2" t="s">
-        <v>53</v>
-      </c>
-      <c r="F2" t="s">
-        <v>77</v>
-      </c>
-      <c r="G2" t="s">
-        <v>66</v>
-      </c>
-      <c r="H2" t="s">
-        <v>62</v>
       </c>
       <c r="I2">
         <v>8</v>
       </c>
       <c r="L2" t="s">
-        <v>110</v>
-      </c>
-      <c r="M2" s="6">
+        <v>106</v>
+      </c>
+      <c r="M2" s="5">
         <v>42504</v>
       </c>
     </row>
-    <row r="3" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>11</v>
       </c>
@@ -1872,22 +1872,22 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="D3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E3" t="s">
+        <v>49</v>
+      </c>
+      <c r="F3" t="s">
+        <v>62</v>
+      </c>
+      <c r="G3" t="s">
+        <v>96</v>
+      </c>
+      <c r="H3" t="s">
         <v>58</v>
-      </c>
-      <c r="E3" t="s">
-        <v>53</v>
-      </c>
-      <c r="F3" t="s">
-        <v>66</v>
-      </c>
-      <c r="G3" t="s">
-        <v>100</v>
-      </c>
-      <c r="H3" t="s">
-        <v>62</v>
       </c>
       <c r="I3">
         <v>8</v>
@@ -1896,13 +1896,13 @@
         <v>4</v>
       </c>
       <c r="L3" t="s">
-        <v>110</v>
-      </c>
-      <c r="M3" s="6">
+        <v>106</v>
+      </c>
+      <c r="M3" s="5">
         <v>42504</v>
       </c>
     </row>
-    <row r="4" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1910,31 +1910,31 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="E4" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="F4" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="G4" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="H4" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="I4">
         <v>6</v>
       </c>
       <c r="L4" t="s">
-        <v>110</v>
-      </c>
-      <c r="M4" s="6">
+        <v>106</v>
+      </c>
+      <c r="M4" s="5">
         <v>42505</v>
       </c>
     </row>
-    <row r="5" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1942,32 +1942,32 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="D5" s="2"/>
       <c r="E5" t="s">
         <v>9</v>
       </c>
       <c r="F5" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="G5" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="H5" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="I5">
         <v>2</v>
       </c>
       <c r="L5" t="s">
-        <v>110</v>
-      </c>
-      <c r="M5" s="6">
+        <v>106</v>
+      </c>
+      <c r="M5" s="5">
         <v>42512</v>
       </c>
     </row>
-    <row r="6" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -1975,31 +1975,31 @@
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E6" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F6" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="G6" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="H6" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="I6">
         <v>6</v>
       </c>
       <c r="L6" t="s">
-        <v>110</v>
-      </c>
-      <c r="M6" s="6">
+        <v>106</v>
+      </c>
+      <c r="M6" s="5">
         <v>42512</v>
       </c>
     </row>
-    <row r="7" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>14</v>
       </c>
@@ -2007,31 +2007,31 @@
         <v>1</v>
       </c>
       <c r="C7" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E7" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="F7" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="G7" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="H7" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="I7">
         <v>2</v>
       </c>
       <c r="L7" t="s">
-        <v>110</v>
-      </c>
-      <c r="M7" s="6">
+        <v>106</v>
+      </c>
+      <c r="M7" s="5">
         <v>42512</v>
       </c>
     </row>
-    <row r="8" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>14</v>
       </c>
@@ -2039,31 +2039,31 @@
         <v>1</v>
       </c>
       <c r="C8" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="E8" t="s">
         <v>9</v>
       </c>
       <c r="F8" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="G8" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="H8" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="I8">
         <v>1</v>
       </c>
       <c r="L8" t="s">
-        <v>110</v>
-      </c>
-      <c r="M8" s="6">
+        <v>106</v>
+      </c>
+      <c r="M8" s="5">
         <v>42512</v>
       </c>
     </row>
-    <row r="9" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>14</v>
       </c>
@@ -2071,31 +2071,31 @@
         <v>1</v>
       </c>
       <c r="C9" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="E9" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F9" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="G9" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="H9" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="I9">
         <v>1</v>
       </c>
       <c r="L9" t="s">
-        <v>110</v>
-      </c>
-      <c r="M9" s="6">
+        <v>106</v>
+      </c>
+      <c r="M9" s="5">
         <v>42512</v>
       </c>
     </row>
-    <row r="10" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1</v>
       </c>
@@ -2103,31 +2103,31 @@
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="E10" t="s">
         <v>9</v>
       </c>
       <c r="F10" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="G10" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="H10" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="I10">
         <v>2</v>
       </c>
       <c r="L10" t="s">
-        <v>110</v>
-      </c>
-      <c r="M10" s="6">
+        <v>106</v>
+      </c>
+      <c r="M10" s="5">
         <v>42512</v>
       </c>
     </row>
-    <row r="11" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>11</v>
       </c>
@@ -2135,31 +2135,31 @@
         <v>1</v>
       </c>
       <c r="C11" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E11" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="F11" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="G11" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="H11" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="I11">
         <v>2</v>
       </c>
       <c r="L11" t="s">
-        <v>110</v>
-      </c>
-      <c r="M11" s="6">
+        <v>106</v>
+      </c>
+      <c r="M11" s="5">
         <v>42505</v>
       </c>
     </row>
-    <row r="12" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>4</v>
       </c>
@@ -2167,19 +2167,19 @@
         <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E12" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="F12" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="G12" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="H12" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="I12">
         <v>6</v>
@@ -2188,13 +2188,13 @@
         <v>4</v>
       </c>
       <c r="L12" t="s">
-        <v>110</v>
-      </c>
-      <c r="M12" s="6">
+        <v>106</v>
+      </c>
+      <c r="M12" s="5">
         <v>42505</v>
       </c>
     </row>
-    <row r="13" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>4</v>
       </c>
@@ -2202,19 +2202,19 @@
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="E13" t="s">
         <v>9</v>
       </c>
       <c r="F13" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="G13" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="H13" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="I13">
         <v>2</v>
@@ -2223,13 +2223,13 @@
         <v>4</v>
       </c>
       <c r="L13" t="s">
-        <v>110</v>
-      </c>
-      <c r="M13" s="6">
+        <v>106</v>
+      </c>
+      <c r="M13" s="5">
         <v>42512</v>
       </c>
     </row>
-    <row r="14" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>4</v>
       </c>
@@ -2237,19 +2237,19 @@
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E14" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F14" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="G14" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="H14" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="I14">
         <v>6</v>
@@ -2258,13 +2258,13 @@
         <v>2</v>
       </c>
       <c r="L14" t="s">
-        <v>110</v>
-      </c>
-      <c r="M14" s="6">
+        <v>106</v>
+      </c>
+      <c r="M14" s="5">
         <v>42512</v>
       </c>
     </row>
-    <row r="15" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>3</v>
       </c>
@@ -2272,31 +2272,31 @@
         <v>2</v>
       </c>
       <c r="C15" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E15" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="F15" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="G15" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="H15" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="I15">
         <v>4</v>
       </c>
       <c r="L15" t="s">
-        <v>110</v>
-      </c>
-      <c r="M15" s="6">
+        <v>106</v>
+      </c>
+      <c r="M15" s="5">
         <v>42519</v>
       </c>
     </row>
-    <row r="16" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>3</v>
       </c>
@@ -2304,34 +2304,34 @@
         <v>2</v>
       </c>
       <c r="C16" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="D16" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="E16" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="F16" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="G16" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="H16" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="I16">
         <v>6</v>
       </c>
       <c r="L16" t="s">
-        <v>110</v>
-      </c>
-      <c r="M16" s="6">
+        <v>106</v>
+      </c>
+      <c r="M16" s="5">
         <v>42519</v>
       </c>
     </row>
-    <row r="17" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>3</v>
       </c>
@@ -2339,34 +2339,34 @@
         <v>2</v>
       </c>
       <c r="C17" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="D17" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E17" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="F17" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="G17" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="H17" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="I17">
         <v>6</v>
       </c>
       <c r="L17" t="s">
-        <v>110</v>
-      </c>
-      <c r="M17" s="6">
+        <v>106</v>
+      </c>
+      <c r="M17" s="5">
         <v>42519</v>
       </c>
     </row>
-    <row r="18" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>2</v>
       </c>
@@ -2374,34 +2374,34 @@
         <v>2</v>
       </c>
       <c r="C18" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D18" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="E18" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="F18" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="G18" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="H18" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="I18">
         <v>4</v>
       </c>
       <c r="L18" t="s">
-        <v>110</v>
-      </c>
-      <c r="M18" s="6">
+        <v>106</v>
+      </c>
+      <c r="M18" s="5">
         <v>42519</v>
       </c>
     </row>
-    <row r="19" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>2</v>
       </c>
@@ -2409,31 +2409,31 @@
         <v>2</v>
       </c>
       <c r="C19" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="E19" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F19" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="G19" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="H19" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="I19">
         <v>5</v>
       </c>
       <c r="L19" t="s">
-        <v>110</v>
-      </c>
-      <c r="M19" s="6">
+        <v>106</v>
+      </c>
+      <c r="M19" s="5">
         <v>42519</v>
       </c>
     </row>
-    <row r="20" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>2</v>
       </c>
@@ -2441,31 +2441,31 @@
         <v>2</v>
       </c>
       <c r="C20" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="E20" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="F20" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="G20" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="H20" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="I20">
         <v>3</v>
       </c>
       <c r="L20" t="s">
-        <v>110</v>
-      </c>
-      <c r="M20" s="6">
+        <v>106</v>
+      </c>
+      <c r="M20" s="5">
         <v>42519</v>
       </c>
     </row>
-    <row r="21" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>15</v>
       </c>
@@ -2473,31 +2473,31 @@
         <v>2</v>
       </c>
       <c r="C21" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="E21" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="F21" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="G21" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="H21" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="I21">
         <v>6</v>
       </c>
       <c r="L21" t="s">
-        <v>110</v>
-      </c>
-      <c r="M21" s="6">
+        <v>106</v>
+      </c>
+      <c r="M21" s="5">
         <v>42519</v>
       </c>
     </row>
-    <row r="22" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>17</v>
       </c>
@@ -2505,31 +2505,31 @@
         <v>2</v>
       </c>
       <c r="C22" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="E22" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="F22" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="G22" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="H22" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="I22">
         <v>10</v>
       </c>
       <c r="L22" t="s">
-        <v>110</v>
-      </c>
-      <c r="M22" s="6">
+        <v>106</v>
+      </c>
+      <c r="M22" s="5">
         <v>42519</v>
       </c>
     </row>
-    <row r="23" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>17</v>
       </c>
@@ -2537,31 +2537,31 @@
         <v>2</v>
       </c>
       <c r="C23" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="E23" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="F23" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="G23" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="H23" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="I23">
         <v>10</v>
       </c>
       <c r="L23" t="s">
-        <v>110</v>
-      </c>
-      <c r="M23" s="6">
+        <v>106</v>
+      </c>
+      <c r="M23" s="5">
         <v>42519</v>
       </c>
     </row>
-    <row r="24" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>16</v>
       </c>
@@ -2569,30 +2569,30 @@
         <v>2</v>
       </c>
       <c r="C24" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="D24" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="E24" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="F24" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="G24" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="H24" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="I24">
         <v>4</v>
       </c>
       <c r="L24" t="s">
-        <v>110</v>
-      </c>
-      <c r="M24" s="6">
+        <v>106</v>
+      </c>
+      <c r="M24" s="5">
         <v>42519</v>
       </c>
     </row>
@@ -2604,30 +2604,27 @@
         <v>3</v>
       </c>
       <c r="C25" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="D25" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="E25" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="F25" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="H25" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="I25">
         <v>3</v>
       </c>
-      <c r="K25">
-        <v>0</v>
-      </c>
       <c r="L25" t="s">
-        <v>171</v>
-      </c>
-      <c r="M25" s="6">
+        <v>106</v>
+      </c>
+      <c r="M25" s="5">
         <v>42535</v>
       </c>
     </row>
@@ -2639,27 +2636,27 @@
         <v>3</v>
       </c>
       <c r="C26" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="D26" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="E26" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="F26" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="H26" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="I26">
         <v>6</v>
       </c>
       <c r="L26" t="s">
-        <v>171</v>
-      </c>
-      <c r="M26" s="6">
+        <v>106</v>
+      </c>
+      <c r="M26" s="5">
         <v>42535</v>
       </c>
     </row>
@@ -2671,27 +2668,27 @@
         <v>3</v>
       </c>
       <c r="C27" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="D27" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="E27" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="F27" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="H27" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="I27">
         <v>6</v>
       </c>
       <c r="L27" t="s">
-        <v>171</v>
-      </c>
-      <c r="M27" s="6">
+        <v>106</v>
+      </c>
+      <c r="M27" s="5">
         <v>42535</v>
       </c>
     </row>
@@ -2703,27 +2700,27 @@
         <v>3</v>
       </c>
       <c r="C28" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="D28" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="E28" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="F28" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="H28" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="I28">
         <v>14</v>
       </c>
       <c r="L28" t="s">
-        <v>171</v>
-      </c>
-      <c r="M28" s="6">
+        <v>106</v>
+      </c>
+      <c r="M28" s="5">
         <v>42535</v>
       </c>
     </row>
@@ -2735,30 +2732,27 @@
         <v>3</v>
       </c>
       <c r="C29" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="D29" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
       <c r="E29" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="F29" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="H29" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="I29">
         <v>10</v>
       </c>
-      <c r="K29">
-        <v>0</v>
-      </c>
       <c r="L29" t="s">
-        <v>171</v>
-      </c>
-      <c r="M29" s="6">
+        <v>106</v>
+      </c>
+      <c r="M29" s="5">
         <v>42535</v>
       </c>
     </row>
@@ -2770,27 +2764,27 @@
         <v>3</v>
       </c>
       <c r="C30" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="D30" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="E30" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="F30" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="H30" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="I30">
         <v>4</v>
       </c>
       <c r="L30" t="s">
-        <v>171</v>
-      </c>
-      <c r="M30" s="6">
+        <v>106</v>
+      </c>
+      <c r="M30" s="5">
         <v>42535</v>
       </c>
     </row>
@@ -2802,24 +2796,24 @@
         <v>3</v>
       </c>
       <c r="C31" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="E31" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F31" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="H31" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="I31">
         <v>4</v>
       </c>
       <c r="L31" t="s">
-        <v>171</v>
-      </c>
-      <c r="M31" s="6">
+        <v>106</v>
+      </c>
+      <c r="M31" s="5">
         <v>42535</v>
       </c>
     </row>
@@ -2831,27 +2825,27 @@
         <v>3</v>
       </c>
       <c r="C32" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="D32" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="E32" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="F32" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="H32" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="I32">
         <v>6</v>
       </c>
       <c r="L32" t="s">
-        <v>171</v>
-      </c>
-      <c r="M32" s="6">
+        <v>106</v>
+      </c>
+      <c r="M32" s="5">
         <v>42535</v>
       </c>
     </row>
@@ -2863,27 +2857,27 @@
         <v>3</v>
       </c>
       <c r="C33" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="D33" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="E33" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="F33" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="H33" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="I33">
         <v>6</v>
       </c>
       <c r="L33" t="s">
-        <v>171</v>
-      </c>
-      <c r="M33" s="6">
+        <v>106</v>
+      </c>
+      <c r="M33" s="5">
         <v>42535</v>
       </c>
     </row>
@@ -2895,28 +2889,28 @@
         <v>3</v>
       </c>
       <c r="C34" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="E34" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="F34" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="H34" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="I34">
         <v>8</v>
       </c>
       <c r="L34" t="s">
-        <v>171</v>
-      </c>
-      <c r="M34" s="6">
+        <v>106</v>
+      </c>
+      <c r="M34" s="5">
         <v>42535</v>
       </c>
     </row>
-    <row r="35" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>18</v>
       </c>
@@ -2924,27 +2918,27 @@
         <v>3</v>
       </c>
       <c r="C35" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="D35" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="E35" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="F35" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="H35" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="I35">
         <v>2</v>
       </c>
       <c r="L35" t="s">
-        <v>110</v>
-      </c>
-      <c r="M35" s="6">
+        <v>106</v>
+      </c>
+      <c r="M35" s="5">
         <v>42535</v>
       </c>
     </row>
@@ -2956,28 +2950,28 @@
         <v>3</v>
       </c>
       <c r="C36" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="E36" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="F36" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="H36" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="I36">
         <v>3</v>
       </c>
       <c r="L36" t="s">
-        <v>171</v>
-      </c>
-      <c r="M36" s="6">
+        <v>106</v>
+      </c>
+      <c r="M36" s="5">
         <v>42535</v>
       </c>
     </row>
-    <row r="37" spans="1:13" hidden="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>18</v>
       </c>
@@ -2985,34 +2979,34 @@
         <v>3</v>
       </c>
       <c r="C37" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="E37" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="F37" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="H37" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="I37">
         <v>2</v>
       </c>
       <c r="L37" t="s">
-        <v>110</v>
-      </c>
-      <c r="M37" s="6">
+        <v>106</v>
+      </c>
+      <c r="M37" s="5">
         <v>42535</v>
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="I38">
         <f>SUBTOTAL(109,Tabelle1[Planned effort])</f>
-        <v>70</v>
+        <v>184</v>
       </c>
     </row>
   </sheetData>
@@ -3025,60 +3019,31 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="10.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" customWidth="1"/>
-    <col min="4" max="4" width="14.33203125" customWidth="1"/>
+    <col min="1" max="1" width="13.5" style="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.1640625" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" style="13" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" style="13" customWidth="1"/>
+    <col min="5" max="16384" width="8.6640625" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="5" customFormat="1" ht="26.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="6">
-        <v>42262</v>
-      </c>
-      <c r="C2">
-        <v>200</v>
-      </c>
-      <c r="D2">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>1</v>
-      </c>
-      <c r="B3" s="6">
-        <v>42263</v>
-      </c>
-      <c r="C3">
-        <v>190</v>
-      </c>
-      <c r="D3">
-        <v>180</v>
-      </c>
+    <row r="1" spans="1:2" s="12" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="15" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B2" s="14"/>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="B3" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>